<commit_message>
my first commit is modified.
</commit_message>
<xml_diff>
--- a/Sheet.xlsx
+++ b/Sheet.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Password</t>
   </si>
@@ -60,9 +60,6 @@
     <t>oneplus 11r mobiile</t>
   </si>
   <si>
-    <t>OnePlus 11R 5G (Galactic Silver, 16GB RAM, 256GB Storage)</t>
-  </si>
-  <si>
     <t>7670969796@axl</t>
   </si>
   <si>
@@ -73,6 +70,12 @@
   </si>
   <si>
     <t>7670969796</t>
+  </si>
+  <si>
+    <t>OnePlus 11R 5G (Sonic Black, 8GB RAM, 128GB Storage)</t>
+  </si>
+  <si>
+    <t>738</t>
   </si>
 </sst>
 </file>
@@ -120,11 +123,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,7 +458,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,17 +501,20 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -512,19 +522,19 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>738</v>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G3" s="2"/>
     </row>

</xml_diff>